<commit_message>
24.12.2021 add fun Revision
</commit_message>
<xml_diff>
--- a/src/main/kotlin/Files/FileAddBom.xlsx
+++ b/src/main/kotlin/Files/FileAddBom.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="43">
   <si>
     <t/>
   </si>
@@ -139,6 +139,15 @@
   </si>
   <si>
     <t>Test</t>
+  </si>
+  <si>
+    <t>B12UA91111213</t>
+  </si>
+  <si>
+    <t>B12UA91111214</t>
+  </si>
+  <si>
+    <t>B12UA91111215</t>
   </si>
 </sst>
 </file>
@@ -578,7 +587,7 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>29</v>
@@ -625,7 +634,7 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>33</v>
@@ -672,7 +681,7 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B4" t="s">
         <v>31</v>
@@ -695,7 +704,7 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B5" t="s">
         <v>25</v>
@@ -718,7 +727,7 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B6" t="s">
         <v>27</v>

</xml_diff>

<commit_message>
27.12.2021 change in fun createNewType, createVersion, CreateRevision
</commit_message>
<xml_diff>
--- a/src/main/kotlin/Files/FileAddBom.xlsx
+++ b/src/main/kotlin/Files/FileAddBom.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="49">
   <si>
     <t/>
   </si>
@@ -148,6 +148,24 @@
   </si>
   <si>
     <t>B12UA91111215</t>
+  </si>
+  <si>
+    <t>B12UAR1111313</t>
+  </si>
+  <si>
+    <t>B12UAR1111314</t>
+  </si>
+  <si>
+    <t>B12UAR1111317</t>
+  </si>
+  <si>
+    <t>B12UAV1111212</t>
+  </si>
+  <si>
+    <t>B12UAX1111212</t>
+  </si>
+  <si>
+    <t>B12UAZ1111212</t>
   </si>
 </sst>
 </file>
@@ -587,7 +605,7 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>29</v>
@@ -634,7 +652,7 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>33</v>
@@ -681,7 +699,7 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="B4" t="s">
         <v>31</v>
@@ -704,7 +722,7 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="B5" t="s">
         <v>25</v>
@@ -727,7 +745,7 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="B6" t="s">
         <v>27</v>

</xml_diff>

<commit_message>
27.12.2021 refactor class EI and Chrome
</commit_message>
<xml_diff>
--- a/src/main/kotlin/Files/FileAddBom.xlsx
+++ b/src/main/kotlin/Files/FileAddBom.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="53">
   <si>
     <t/>
   </si>
@@ -169,6 +169,15 @@
   </si>
   <si>
     <t>B12UB21111212</t>
+  </si>
+  <si>
+    <t>B12UB31111212</t>
+  </si>
+  <si>
+    <t>B12UB41111212</t>
+  </si>
+  <si>
+    <t>B12UB51111212</t>
   </si>
 </sst>
 </file>
@@ -608,7 +617,7 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>29</v>
@@ -655,7 +664,7 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>33</v>
@@ -702,7 +711,7 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B4" t="s">
         <v>31</v>
@@ -725,7 +734,7 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B5" t="s">
         <v>25</v>
@@ -748,7 +757,7 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B6" t="s">
         <v>27</v>

</xml_diff>